<commit_message>
Manually edited global csv files
</commit_message>
<xml_diff>
--- a/docs/vision_global_anuales.xlsx
+++ b/docs/vision_global_anuales.xlsx
@@ -43,19 +43,19 @@
     <t xml:space="preserve"> - Indicadores</t>
   </si>
   <si>
-    <t xml:space="preserve">España - 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">España - 2017</t>
+    <t xml:space="preserve">España – 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España – 2015</t>
   </si>
   <si>
     <t xml:space="preserve">España - 2016</t>
   </si>
   <si>
-    <t xml:space="preserve">España - 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">España - 2014</t>
+    <t xml:space="preserve">España – 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">España – 2018</t>
   </si>
   <si>
     <t xml:space="preserve">Economía</t>
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -178,7 +179,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>